<commit_message>
Deploying to gh-pages from @ Alvearie/alvearie-fhir-ig@b468df15829f65ba3bd6bf1a0a8a10aa45b2ef81 🚀
</commit_message>
<xml_diff>
--- a/0.1.0/StructureDefinition-cdm-coverage.xlsx
+++ b/0.1.0/StructureDefinition-cdm-coverage.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$71</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2531" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="384">
   <si>
     <t>Path</t>
   </si>
@@ -383,6 +383,16 @@
     <t>Standard code for groupings that combine age and gender</t>
   </si>
   <si>
+    <t>coverageDays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/coverage-days}
+</t>
+  </si>
+  <si>
+    <t>The number of covered days of eligibility</t>
+  </si>
+  <si>
     <t>coverageMonth</t>
   </si>
   <si>
@@ -393,6 +403,16 @@
     <t>The date which reflects the month of eligibility</t>
   </si>
   <si>
+    <t>coverageInsurancePlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/coverage-insurance-plan}
+</t>
+  </si>
+  <si>
+    <t>The insurance plan providing coverage</t>
+  </si>
+  <si>
     <t>enrollmentPcp</t>
   </si>
   <si>
@@ -527,6 +547,16 @@
   </si>
   <si>
     <t>Indicates whether the member is either an employee of the health plan, or the dependent of an employee of the health plan</t>
+  </si>
+  <si>
+    <t>regionCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/region-code}
+</t>
+  </si>
+  <si>
+    <t>Customer-specific code for the geographic region of the employee</t>
   </si>
   <si>
     <t>attributedProviderReferenceWithPeriod</t>
@@ -1344,7 +1374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO68"/>
+  <dimension ref="A1:AO71"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3186,7 +3216,7 @@
         <v>124</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -3275,7 +3305,7 @@
         <v>96</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s" s="2">
         <v>42</v>
@@ -3297,13 +3327,13 @@
         <v>42</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>127</v>
       </c>
-      <c r="K17" t="s" s="2">
-        <v>128</v>
-      </c>
       <c r="L17" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -3392,7 +3422,7 @@
         <v>96</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>42</v>
@@ -3414,13 +3444,13 @@
         <v>42</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>130</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>131</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>132</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3509,7 +3539,7 @@
         <v>96</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s" s="2">
         <v>42</v>
@@ -3531,13 +3561,13 @@
         <v>42</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>134</v>
       </c>
-      <c r="K19" t="s" s="2">
-        <v>135</v>
-      </c>
       <c r="L19" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3626,7 +3656,7 @@
         <v>96</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s" s="2">
         <v>42</v>
@@ -3648,10 +3678,10 @@
         <v>42</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>137</v>
-      </c>
-      <c r="K20" t="s" s="2">
-        <v>138</v>
       </c>
       <c r="L20" t="s" s="2">
         <v>138</v>
@@ -4707,7 +4737,7 @@
         <v>165</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4796,7 +4826,7 @@
         <v>96</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>42</v>
@@ -4818,13 +4848,13 @@
         <v>42</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="K30" t="s" s="2">
-        <v>169</v>
-      </c>
       <c r="L30" t="s" s="2">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4913,7 +4943,7 @@
         <v>96</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C31" t="s" s="2">
         <v>42</v>
@@ -4935,13 +4965,13 @@
         <v>42</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5030,7 +5060,7 @@
         <v>96</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>42</v>
@@ -5052,13 +5082,13 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="K32" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>175</v>
-      </c>
-      <c r="K32" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>176</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5147,7 +5177,7 @@
         <v>96</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>42</v>
@@ -5169,10 +5199,10 @@
         <v>42</v>
       </c>
       <c r="J33" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="K33" t="s" s="2">
         <v>178</v>
-      </c>
-      <c r="K33" t="s" s="2">
-        <v>179</v>
       </c>
       <c r="L33" t="s" s="2">
         <v>179</v>
@@ -5261,43 +5291,41 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>42</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I34" t="s" s="2">
         <v>42</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>97</v>
+        <v>181</v>
       </c>
       <c r="K34" t="s" s="2">
         <v>182</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>185</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>42</v>
       </c>
@@ -5345,7 +5373,7 @@
         <v>42</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>186</v>
+        <v>102</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5354,7 +5382,7 @@
         <v>44</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>103</v>
@@ -5380,9 +5408,11 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="B35" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="B35" t="s" s="2">
+        <v>183</v>
+      </c>
       <c r="C35" t="s" s="2">
         <v>42</v>
       </c>
@@ -5391,7 +5421,7 @@
         <v>43</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>42</v>
@@ -5403,20 +5433,16 @@
         <v>42</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>192</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>42</v>
       </c>
@@ -5464,7 +5490,7 @@
         <v>42</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>187</v>
+        <v>102</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5476,13 +5502,13 @@
         <v>63</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>193</v>
+        <v>65</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>42</v>
@@ -5491,7 +5517,7 @@
         <v>42</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>194</v>
+        <v>42</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>42</v>
@@ -5499,15 +5525,17 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="B36" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="B36" t="s" s="2">
+        <v>186</v>
+      </c>
       <c r="C36" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>51</v>
@@ -5516,26 +5544,22 @@
         <v>42</v>
       </c>
       <c r="H36" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>73</v>
+        <v>187</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>199</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>42</v>
       </c>
@@ -5559,13 +5583,13 @@
         <v>42</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>200</v>
+        <v>42</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>201</v>
+        <v>42</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>42</v>
@@ -5583,28 +5607,28 @@
         <v>42</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>195</v>
+        <v>102</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>203</v>
+        <v>42</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>204</v>
+        <v>65</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>205</v>
+        <v>42</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>42</v>
@@ -5618,40 +5642,42 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>42</v>
       </c>
       <c r="H37" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>207</v>
+        <v>97</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="M37" s="2"/>
+        <v>192</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>193</v>
+      </c>
       <c r="N37" t="s" s="2">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>42</v>
@@ -5676,13 +5702,13 @@
         <v>42</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>211</v>
+        <v>42</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>212</v>
+        <v>42</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>42</v>
@@ -5700,34 +5726,34 @@
         <v>42</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>213</v>
+        <v>42</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>214</v>
+        <v>42</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>42</v>
@@ -5735,7 +5761,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5746,7 +5772,7 @@
         <v>43</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>42</v>
@@ -5755,22 +5781,22 @@
         <v>42</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>42</v>
@@ -5819,16 +5845,16 @@
         <v>42</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>64</v>
@@ -5837,24 +5863,24 @@
         <v>42</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>42</v>
+        <v>202</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>221</v>
+        <v>42</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>222</v>
+        <v>42</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>224</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5862,7 +5888,7 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F39" t="s" s="2">
         <v>51</v>
@@ -5871,25 +5897,25 @@
         <v>42</v>
       </c>
       <c r="H39" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I39" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>226</v>
+        <v>73</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>42</v>
@@ -5914,13 +5940,13 @@
         <v>42</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>42</v>
+        <v>209</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>42</v>
+        <v>210</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>42</v>
+        <v>211</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>42</v>
@@ -5938,10 +5964,10 @@
         <v>42</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>51</v>
@@ -5953,27 +5979,27 @@
         <v>64</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>42</v>
+        <v>212</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>42</v>
+        <v>213</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>222</v>
+        <v>42</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>223</v>
+        <v>42</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>224</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5996,17 +6022,17 @@
         <v>52</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>53</v>
+        <v>216</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" t="s" s="2">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>42</v>
@@ -6031,13 +6057,13 @@
         <v>42</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>42</v>
+        <v>220</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>42</v>
+        <v>221</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>42</v>
@@ -6055,7 +6081,7 @@
         <v>42</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6076,21 +6102,21 @@
         <v>42</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>222</v>
+        <v>42</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>223</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>224</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6098,7 +6124,7 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F41" t="s" s="2">
         <v>51</v>
@@ -6113,17 +6139,19 @@
         <v>52</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="M41" s="2"/>
+        <v>227</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>228</v>
+      </c>
       <c r="N41" t="s" s="2">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>42</v>
@@ -6172,10 +6200,10 @@
         <v>42</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>51</v>
@@ -6187,27 +6215,27 @@
         <v>64</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>240</v>
+        <v>42</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>224</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6230,19 +6258,19 @@
         <v>52</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>53</v>
+        <v>235</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>42</v>
@@ -6291,7 +6319,7 @@
         <v>42</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6312,21 +6340,21 @@
         <v>42</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>42</v>
+        <v>230</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="AO42" t="s" s="2">
-        <v>42</v>
+        <v>233</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6346,22 +6374,20 @@
         <v>42</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>207</v>
+        <v>53</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>251</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="M43" s="2"/>
       <c r="N43" t="s" s="2">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>42</v>
@@ -6386,13 +6412,13 @@
         <v>42</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>253</v>
+        <v>42</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>254</v>
+        <v>42</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>255</v>
+        <v>42</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>42</v>
@@ -6410,7 +6436,7 @@
         <v>42</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6431,21 +6457,21 @@
         <v>42</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>42</v>
+        <v>230</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>42</v>
+        <v>232</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>42</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6468,17 +6494,17 @@
         <v>52</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" t="s" s="2">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>42</v>
@@ -6527,10 +6553,10 @@
         <v>42</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>51</v>
@@ -6542,27 +6568,27 @@
         <v>64</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>263</v>
+        <v>42</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>42</v>
+        <v>231</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>265</v>
+        <v>232</v>
       </c>
       <c r="AO44" t="s" s="2">
-        <v>42</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6570,7 +6596,7 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
         <v>51</v>
@@ -6585,19 +6611,19 @@
         <v>52</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>267</v>
+        <v>53</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>42</v>
@@ -6646,13 +6672,13 @@
         <v>42</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="AF45" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG45" t="s" s="2">
         <v>51</v>
-      </c>
-      <c r="AG45" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>42</v>
@@ -6667,21 +6693,21 @@
         <v>42</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>272</v>
+        <v>42</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="AO45" t="s" s="2">
-        <v>275</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6692,7 +6718,7 @@
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>42</v>
@@ -6704,19 +6730,19 @@
         <v>42</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>277</v>
+        <v>216</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>42</v>
@@ -6741,13 +6767,13 @@
         <v>42</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>42</v>
+        <v>262</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>42</v>
+        <v>263</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>42</v>
@@ -6765,13 +6791,13 @@
         <v>42</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>42</v>
@@ -6789,7 +6815,7 @@
         <v>42</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>42</v>
+        <v>265</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>42</v>
@@ -6800,7 +6826,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6808,7 +6834,7 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F47" t="s" s="2">
         <v>51</v>
@@ -6820,19 +6846,21 @@
         <v>42</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>53</v>
+        <v>267</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
+      <c r="N47" t="s" s="2">
+        <v>270</v>
+      </c>
       <c r="O47" t="s" s="2">
         <v>42</v>
       </c>
@@ -6880,7 +6908,7 @@
         <v>42</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -6892,22 +6920,22 @@
         <v>42</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>42</v>
+        <v>271</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>42</v>
+        <v>273</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>42</v>
+        <v>274</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>42</v>
@@ -6915,18 +6943,18 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>42</v>
@@ -6935,21 +6963,23 @@
         <v>42</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>97</v>
+        <v>276</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="N48" s="2"/>
+        <v>279</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="O48" t="s" s="2">
         <v>42</v>
       </c>
@@ -6997,10 +7027,10 @@
         <v>42</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>44</v>
@@ -7009,34 +7039,34 @@
         <v>42</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>286</v>
+        <v>42</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>42</v>
+        <v>281</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>42</v>
+        <v>282</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>42</v>
+        <v>283</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>42</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>292</v>
+        <v>42</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -7049,25 +7079,25 @@
         <v>42</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I49" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>97</v>
+        <v>286</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>184</v>
+        <v>289</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>185</v>
+        <v>290</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>42</v>
@@ -7116,7 +7146,7 @@
         <v>42</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7128,13 +7158,13 @@
         <v>42</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>42</v>
@@ -7151,7 +7181,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7159,7 +7189,7 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>51</v>
@@ -7171,21 +7201,19 @@
         <v>42</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>207</v>
+        <v>53</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="M50" s="2"/>
-      <c r="N50" t="s" s="2">
-        <v>299</v>
-      </c>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>42</v>
       </c>
@@ -7209,13 +7237,13 @@
         <v>42</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>253</v>
+        <v>42</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>300</v>
+        <v>42</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>301</v>
+        <v>42</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>42</v>
@@ -7233,10 +7261,10 @@
         <v>42</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>51</v>
@@ -7245,13 +7273,13 @@
         <v>42</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>42</v>
+        <v>295</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>42</v>
@@ -7268,18 +7296,18 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>42</v>
@@ -7288,23 +7316,21 @@
         <v>42</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>306</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>42</v>
       </c>
@@ -7352,75 +7378,77 @@
         <v>42</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>42</v>
+        <v>295</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>307</v>
+        <v>42</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>308</v>
+        <v>42</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>309</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>42</v>
+        <v>301</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>42</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I52" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="M52" s="2"/>
+        <v>303</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>193</v>
+      </c>
       <c r="N52" t="s" s="2">
-        <v>313</v>
+        <v>194</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>42</v>
@@ -7469,42 +7497,42 @@
         <v>42</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>307</v>
+        <v>42</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>308</v>
+        <v>42</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>309</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7512,7 +7540,7 @@
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F53" t="s" s="2">
         <v>51</v>
@@ -7527,17 +7555,17 @@
         <v>52</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>315</v>
+        <v>216</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" t="s" s="2">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>42</v>
@@ -7562,13 +7590,13 @@
         <v>42</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>42</v>
+        <v>262</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>42</v>
+        <v>309</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>42</v>
+        <v>310</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>42</v>
@@ -7586,10 +7614,10 @@
         <v>42</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>51</v>
@@ -7613,7 +7641,7 @@
         <v>42</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>247</v>
+        <v>42</v>
       </c>
       <c r="AO53" t="s" s="2">
         <v>42</v>
@@ -7621,7 +7649,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7629,7 +7657,7 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F54" t="s" s="2">
         <v>51</v>
@@ -7647,14 +7675,16 @@
         <v>53</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="M54" s="2"/>
+        <v>313</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>314</v>
+      </c>
       <c r="N54" t="s" s="2">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>42</v>
@@ -7703,10 +7733,10 @@
         <v>42</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>51</v>
@@ -7727,29 +7757,29 @@
         <v>42</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>42</v>
+        <v>317</v>
       </c>
       <c r="AO54" t="s" s="2">
-        <v>42</v>
+        <v>318</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>325</v>
+        <v>42</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F55" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G55" t="s" s="2">
         <v>42</v>
@@ -7758,22 +7788,20 @@
         <v>42</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>277</v>
+        <v>53</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>328</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>42</v>
@@ -7822,13 +7850,13 @@
         <v>42</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG55" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="AH55" t="s" s="2">
         <v>42</v>
@@ -7846,18 +7874,18 @@
         <v>42</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>42</v>
+        <v>316</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>42</v>
+        <v>317</v>
       </c>
       <c r="AO55" t="s" s="2">
-        <v>42</v>
+        <v>318</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7877,19 +7905,21 @@
         <v>42</v>
       </c>
       <c r="I56" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>53</v>
+        <v>324</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>283</v>
+        <v>325</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>284</v>
+        <v>326</v>
       </c>
       <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
+      <c r="N56" t="s" s="2">
+        <v>327</v>
+      </c>
       <c r="O56" t="s" s="2">
         <v>42</v>
       </c>
@@ -7937,7 +7967,7 @@
         <v>42</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>285</v>
+        <v>323</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -7949,13 +7979,13 @@
         <v>42</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>286</v>
+        <v>42</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>42</v>
@@ -7964,7 +7994,7 @@
         <v>42</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>42</v>
+        <v>256</v>
       </c>
       <c r="AO56" t="s" s="2">
         <v>42</v>
@@ -7972,18 +8002,18 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G57" t="s" s="2">
         <v>42</v>
@@ -7992,21 +8022,21 @@
         <v>42</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>288</v>
+        <v>329</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="N57" s="2"/>
+        <v>330</v>
+      </c>
+      <c r="M57" s="2"/>
+      <c r="N57" t="s" s="2">
+        <v>331</v>
+      </c>
       <c r="O57" t="s" s="2">
         <v>42</v>
       </c>
@@ -8054,31 +8084,31 @@
         <v>42</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>290</v>
+        <v>328</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG57" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="AH57" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ57" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>286</v>
+        <v>42</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>42</v>
+        <v>332</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>42</v>
@@ -8089,11 +8119,11 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>292</v>
+        <v>334</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8106,25 +8136,25 @@
         <v>42</v>
       </c>
       <c r="H58" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>97</v>
+        <v>286</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>293</v>
+        <v>335</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>294</v>
+        <v>336</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>184</v>
+        <v>337</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>185</v>
+        <v>338</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>42</v>
@@ -8173,7 +8203,7 @@
         <v>42</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>295</v>
+        <v>333</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
@@ -8185,13 +8215,13 @@
         <v>42</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>42</v>
@@ -8208,7 +8238,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8228,23 +8258,19 @@
         <v>42</v>
       </c>
       <c r="I59" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>207</v>
+        <v>53</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>337</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>42</v>
       </c>
@@ -8268,13 +8294,13 @@
         <v>42</v>
       </c>
       <c r="W59" t="s" s="2">
-        <v>253</v>
+        <v>42</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>338</v>
+        <v>42</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>339</v>
+        <v>42</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>42</v>
@@ -8292,7 +8318,7 @@
         <v>42</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>333</v>
+        <v>294</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8304,13 +8330,13 @@
         <v>42</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="AJ59" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>42</v>
+        <v>295</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>42</v>
@@ -8331,14 +8357,14 @@
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>42</v>
@@ -8347,23 +8373,21 @@
         <v>42</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>341</v>
+        <v>97</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>342</v>
+        <v>297</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>343</v>
+        <v>298</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>345</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>42</v>
       </c>
@@ -8411,46 +8435,46 @@
         <v>42</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>340</v>
+        <v>299</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>42</v>
+        <v>295</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>307</v>
+        <v>42</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>308</v>
+        <v>42</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>309</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>42</v>
+        <v>301</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
@@ -8463,23 +8487,25 @@
         <v>42</v>
       </c>
       <c r="H61" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I61" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>277</v>
+        <v>97</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>347</v>
+        <v>302</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="M61" s="2"/>
+        <v>303</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>193</v>
+      </c>
       <c r="N61" t="s" s="2">
-        <v>329</v>
+        <v>194</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>42</v>
@@ -8528,7 +8554,7 @@
         <v>42</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>346</v>
+        <v>304</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
@@ -8540,13 +8566,13 @@
         <v>42</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>42</v>
@@ -8563,7 +8589,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8583,19 +8609,23 @@
         <v>42</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>53</v>
+        <v>216</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>283</v>
+        <v>343</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
+        <v>344</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="N62" t="s" s="2">
+        <v>346</v>
+      </c>
       <c r="O62" t="s" s="2">
         <v>42</v>
       </c>
@@ -8619,13 +8649,13 @@
         <v>42</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>42</v>
+        <v>262</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>42</v>
+        <v>347</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>42</v>
+        <v>348</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>42</v>
@@ -8643,7 +8673,7 @@
         <v>42</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>285</v>
+        <v>342</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -8655,13 +8685,13 @@
         <v>42</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>286</v>
+        <v>42</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>42</v>
@@ -8678,18 +8708,18 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F63" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>42</v>
@@ -8698,21 +8728,23 @@
         <v>42</v>
       </c>
       <c r="I63" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>97</v>
+        <v>350</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>288</v>
+        <v>351</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>289</v>
+        <v>352</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="N63" s="2"/>
+        <v>353</v>
+      </c>
+      <c r="N63" t="s" s="2">
+        <v>354</v>
+      </c>
       <c r="O63" t="s" s="2">
         <v>42</v>
       </c>
@@ -8760,46 +8792,46 @@
         <v>42</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>290</v>
+        <v>349</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AG63" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="AH63" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ63" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>286</v>
+        <v>42</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>42</v>
+        <v>316</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>42</v>
+        <v>317</v>
       </c>
       <c r="AO63" t="s" s="2">
-        <v>42</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>292</v>
+        <v>42</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
@@ -8812,25 +8844,23 @@
         <v>42</v>
       </c>
       <c r="H64" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I64" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>97</v>
+        <v>286</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>293</v>
+        <v>356</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>184</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="M64" s="2"/>
       <c r="N64" t="s" s="2">
-        <v>185</v>
+        <v>338</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>42</v>
@@ -8879,7 +8909,7 @@
         <v>42</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>295</v>
+        <v>355</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
@@ -8891,13 +8921,13 @@
         <v>42</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ64" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>42</v>
@@ -8914,7 +8944,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8922,7 +8952,7 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F65" t="s" s="2">
         <v>51</v>
@@ -8934,21 +8964,19 @@
         <v>42</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>207</v>
+        <v>53</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>353</v>
+        <v>292</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>354</v>
+        <v>293</v>
       </c>
       <c r="M65" s="2"/>
-      <c r="N65" t="s" s="2">
-        <v>355</v>
-      </c>
+      <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>42</v>
       </c>
@@ -8972,13 +9000,13 @@
         <v>42</v>
       </c>
       <c r="W65" t="s" s="2">
-        <v>356</v>
+        <v>42</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>357</v>
+        <v>42</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>358</v>
+        <v>42</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>42</v>
@@ -8996,10 +9024,10 @@
         <v>42</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>352</v>
+        <v>294</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>51</v>
@@ -9008,13 +9036,13 @@
         <v>42</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>42</v>
+        <v>295</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>42</v>
@@ -9035,14 +9063,14 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>42</v>
@@ -9051,21 +9079,21 @@
         <v>42</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>258</v>
+        <v>97</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>360</v>
+        <v>297</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="M66" s="2"/>
-      <c r="N66" t="s" s="2">
-        <v>362</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>42</v>
       </c>
@@ -9113,25 +9141,25 @@
         <v>42</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>359</v>
+        <v>299</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>42</v>
+        <v>295</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>42</v>
@@ -9148,42 +9176,42 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>42</v>
+        <v>301</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G67" t="s" s="2">
         <v>42</v>
       </c>
       <c r="H67" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I67" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>364</v>
+        <v>97</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>365</v>
+        <v>302</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>366</v>
+        <v>303</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>367</v>
+        <v>193</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>368</v>
+        <v>194</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>42</v>
@@ -9232,25 +9260,25 @@
         <v>42</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>363</v>
+        <v>304</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG67" t="s" s="2">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AH67" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>42</v>
@@ -9267,7 +9295,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9275,10 +9303,10 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G68" t="s" s="2">
         <v>42</v>
@@ -9287,20 +9315,20 @@
         <v>42</v>
       </c>
       <c r="I68" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>370</v>
+        <v>216</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" t="s" s="2">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>42</v>
@@ -9325,13 +9353,13 @@
         <v>42</v>
       </c>
       <c r="W68" t="s" s="2">
-        <v>42</v>
+        <v>365</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>42</v>
+        <v>366</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>42</v>
+        <v>367</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>42</v>
@@ -9349,13 +9377,13 @@
         <v>42</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="AH68" t="s" s="2">
         <v>42</v>
@@ -9367,23 +9395,376 @@
         <v>42</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>286</v>
+        <v>42</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>222</v>
+        <v>42</v>
       </c>
       <c r="AN68" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AO68" t="s" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" hidden="true">
+      <c r="A69" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F69" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I69" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J69" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="K69" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="L69" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="M69" s="2"/>
+      <c r="N69" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="O69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="P69" s="2"/>
+      <c r="Q69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE69" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AF69" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG69" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI69" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AJ69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AK69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AM69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AN69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AO69" t="s" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" hidden="true">
+      <c r="A70" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F70" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="J70" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="K70" t="s" s="2">
         <v>374</v>
       </c>
-      <c r="AO68" t="s" s="2">
-        <v>224</v>
+      <c r="L70" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="M70" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="N70" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="O70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="P70" s="2"/>
+      <c r="Q70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE70" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="AF70" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG70" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI70" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AJ70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AK70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AM70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AN70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AO70" t="s" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" hidden="true">
+      <c r="A71" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="J71" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="K71" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="L71" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="M71" s="2"/>
+      <c r="N71" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="O71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="P71" s="2"/>
+      <c r="Q71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE71" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="AF71" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI71" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AJ71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AK71" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AL71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AM71" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="AN71" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="AO71" t="s" s="2">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO68">
+  <autoFilter ref="A1:AO71">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -9393,7 +9774,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI67">
+  <conditionalFormatting sqref="A2:AI70">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>